<commit_message>
misorientations working, tweaking stats now
</commit_message>
<xml_diff>
--- a/src/stats.xlsx
+++ b/src/stats.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\crystal\src\neper_gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\crystal\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56A0B2C-E2BB-4EC7-BD6F-80ECCF99B309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF951F6E-B30F-4938-A82D-30C04C1BF9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
-    <sheet name="temp" sheetId="2" r:id="rId2"/>
-    <sheet name="time" sheetId="3" r:id="rId3"/>
-    <sheet name="time2" sheetId="4" r:id="rId4"/>
+    <sheet name="time" sheetId="3" r:id="rId2"/>
+    <sheet name="time2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>twins</t>
   </si>
@@ -49,9 +48,6 @@
     <t>thickness</t>
   </si>
   <si>
-    <t>length</t>
-  </si>
-  <si>
     <t>sphericity</t>
   </si>
   <si>
@@ -59,9 +55,6 @@
   </si>
   <si>
     <t>mu</t>
-  </si>
-  <si>
-    <t>sig</t>
   </si>
   <si>
     <t>equiv. radius</t>
@@ -92,6 +85,12 @@
   </si>
   <si>
     <t>mesh time around 10 times tessellation</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -259,16 +258,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8433,41 +8432,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="2" customWidth="1"/>
-    <col min="5" max="9" width="8.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="8" customWidth="1"/>
+    <col min="2" max="4" width="8.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="2" customWidth="1"/>
+    <col min="7" max="11" width="8.7109375" style="6" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="6" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="8" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="1"/>
+    <col min="15" max="15" width="8.7109375" style="6" customWidth="1"/>
+    <col min="16" max="18" width="8.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" style="6" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
@@ -8477,681 +8476,385 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="15"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="13" t="s">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
+      <c r="G3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.3788</v>
       </c>
       <c r="B4" s="2">
         <v>0.88415999999999995</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
+        <v>0.51841000000000004</v>
+      </c>
+      <c r="D4" s="2">
+        <v>69.183400000000006</v>
+      </c>
+      <c r="E4" s="1">
         <v>5.8689999999999998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>40.825899999999997</v>
       </c>
-      <c r="E4" s="8">
+      <c r="G4" s="6">
         <v>4.3425000000000002</v>
       </c>
-      <c r="F4" s="8">
+      <c r="H4" s="6">
         <v>1.0053000000000001</v>
       </c>
-      <c r="G4" s="8">
+      <c r="I4" s="6">
         <v>127.4554</v>
       </c>
-      <c r="H4" s="8">
+      <c r="J4" s="6">
         <v>28384.641199999998</v>
       </c>
-      <c r="I4" s="8">
+      <c r="K4" s="6">
         <v>-0.95459000000000005</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>0.13492000000000001</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="6">
         <v>0.38849</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>2.7726999999999999E-3</v>
       </c>
-      <c r="M4" s="8">
+      <c r="O4" s="6">
         <v>2.9203000000000001</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>1.2495000000000001</v>
       </c>
-      <c r="O4" s="8">
+      <c r="Q4" s="2">
+        <v>1.6969000000000001</v>
+      </c>
+      <c r="R4" s="2">
+        <v>215.10939999999999</v>
+      </c>
+      <c r="S4" s="6">
         <v>40.483600000000003</v>
       </c>
-      <c r="P4" s="2">
+      <c r="T4" s="2">
         <v>6170.0387000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.5431999999999999</v>
       </c>
       <c r="B5" s="2">
         <v>0.81201999999999996</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
+        <v>0.86428000000000005</v>
+      </c>
+      <c r="D5" s="2">
+        <v>41.155099999999997</v>
+      </c>
+      <c r="E5" s="1">
         <v>6.5071000000000003</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <v>39.530500000000004</v>
       </c>
-      <c r="E5" s="8">
+      <c r="G5" s="6">
         <v>3.8673000000000002</v>
       </c>
-      <c r="F5" s="8">
+      <c r="H5" s="6">
         <v>1.3140000000000001</v>
       </c>
-      <c r="G5" s="8">
+      <c r="I5" s="6">
         <v>113.3644</v>
       </c>
-      <c r="H5" s="8">
+      <c r="J5" s="6">
         <v>59399.080900000001</v>
       </c>
-      <c r="I5" s="8">
+      <c r="K5" s="6">
         <v>-0.98540000000000005</v>
       </c>
-      <c r="J5" s="2">
+      <c r="L5" s="2">
         <v>0.13211999999999999</v>
       </c>
-      <c r="K5" s="8">
+      <c r="M5" s="6">
         <v>0.37656000000000001</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>2.4968E-3</v>
       </c>
-      <c r="M5" s="8">
+      <c r="O5" s="6">
         <v>3.2942</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>1.03</v>
       </c>
-      <c r="O5" s="8">
+      <c r="Q5" s="2">
+        <v>2.7725</v>
+      </c>
+      <c r="R5" s="2">
+        <v>191.77359999999999</v>
+      </c>
+      <c r="S5" s="6">
         <v>45.819400000000002</v>
       </c>
-      <c r="P5" s="2">
+      <c r="T5" s="2">
         <v>3965.8737000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.4343999999999999</v>
       </c>
       <c r="B6" s="2">
         <v>0.93140999999999996</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
+        <v>0.42991000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>69.313299999999998</v>
+      </c>
+      <c r="E6" s="1">
         <v>6.4763000000000002</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>57.923499999999997</v>
       </c>
-      <c r="E6" s="8">
+      <c r="G6" s="6">
         <v>3.9472999999999998</v>
       </c>
-      <c r="F6" s="8">
+      <c r="H6" s="6">
         <v>1.2231000000000001</v>
       </c>
-      <c r="G6" s="8">
+      <c r="I6" s="6">
         <v>109.42529999999999</v>
       </c>
-      <c r="H6" s="8">
+      <c r="J6" s="6">
         <v>41469.869299999998</v>
       </c>
-      <c r="I6" s="8">
+      <c r="K6" s="6">
         <v>-0.94411999999999996</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>0.12615999999999999</v>
       </c>
-      <c r="K6" s="8">
+      <c r="M6" s="6">
         <v>0.39212999999999998</v>
       </c>
-      <c r="L6" s="2">
+      <c r="N6" s="2">
         <v>2.4670999999999998E-3</v>
       </c>
-      <c r="M6" s="8">
+      <c r="O6" s="6">
         <v>2.8203</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>1.3335999999999999</v>
       </c>
-      <c r="O6" s="8">
+      <c r="Q6" s="2">
+        <v>1.6354</v>
+      </c>
+      <c r="R6" s="2">
+        <v>257.05889999999999</v>
+      </c>
+      <c r="S6" s="6">
         <v>40.837699999999998</v>
       </c>
-      <c r="P6" s="2">
+      <c r="T6" s="2">
         <v>8207.7829000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f>AVERAGE(A4:A6)</f>
         <v>1.4521333333333333</v>
       </c>
-      <c r="B7" s="6">
-        <f t="shared" ref="B7:H7" si="0">AVERAGE(B4:B6)</f>
+      <c r="B7" s="5">
+        <f t="shared" ref="B7:J7" si="0">AVERAGE(B4:B6)</f>
         <v>0.87586333333333333</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="9">
+        <f t="shared" ref="C7" si="1">AVERAGE(C4:C6)</f>
+        <v>0.60420000000000007</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ref="D7" si="2">AVERAGE(D4:D6)</f>
+        <v>59.883933333333339</v>
+      </c>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>6.284133333333334</v>
       </c>
-      <c r="D7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>46.093299999999999</v>
       </c>
-      <c r="E7" s="9">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>4.0523666666666669</v>
       </c>
-      <c r="F7" s="9">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>1.1808000000000001</v>
       </c>
-      <c r="G7" s="9">
+      <c r="I7" s="7">
         <f t="shared" si="0"/>
         <v>116.74836666666666</v>
       </c>
-      <c r="H7" s="9">
+      <c r="J7" s="7">
         <f t="shared" si="0"/>
         <v>43084.530466666671</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" ref="I7" si="1">AVERAGE(I4:I6)</f>
+      <c r="K7" s="3">
+        <f t="shared" ref="K7" si="3">AVERAGE(K4:K6)</f>
         <v>-0.96137000000000006</v>
       </c>
-      <c r="J7" s="6">
-        <f t="shared" ref="J7:P7" si="2">AVERAGE(J4:J6)</f>
+      <c r="L7" s="5">
+        <f t="shared" ref="L7:T7" si="4">AVERAGE(L4:L6)</f>
         <v>0.13106666666666666</v>
       </c>
-      <c r="K7" s="6">
-        <f t="shared" si="2"/>
+      <c r="M7" s="5">
+        <f t="shared" si="4"/>
         <v>0.38572666666666661</v>
       </c>
-      <c r="L7" s="6">
-        <f t="shared" si="2"/>
+      <c r="N7" s="5">
+        <f t="shared" si="4"/>
         <v>2.5788666666666667E-3</v>
       </c>
-      <c r="M7" s="6">
-        <f t="shared" si="2"/>
+      <c r="O7" s="5">
+        <f t="shared" si="4"/>
         <v>3.0116000000000001</v>
       </c>
-      <c r="N7" s="6">
-        <f t="shared" si="2"/>
+      <c r="P7" s="5">
+        <f t="shared" si="4"/>
         <v>1.2043666666666668</v>
       </c>
-      <c r="O7" s="6">
-        <f t="shared" si="2"/>
+      <c r="Q7" s="9">
+        <f t="shared" ref="Q7:R7" si="5">AVERAGE(Q4:Q6)</f>
+        <v>2.0349333333333335</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="5"/>
+        <v>221.31396666666669</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="4"/>
         <v>42.380233333333329</v>
       </c>
-      <c r="P7" s="6">
-        <f t="shared" si="2"/>
+      <c r="T7" s="5">
+        <f t="shared" si="4"/>
         <v>6114.5650999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="E1:P1"/>
-    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="G1:T1"/>
+    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054C0814-E2C3-4FDA-BFAD-EE4274AEE67E}">
-  <dimension ref="A1:P7"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="8" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="8" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="15"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.3788</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.88415999999999995</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2.8839000000000001</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.84709999999999996</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-1.2455000000000001</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.25973000000000002</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2.1314000000000002</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.80762999999999996</v>
-      </c>
-      <c r="I4" s="1">
-        <v>3.6255999999999999</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.84616000000000002</v>
-      </c>
-      <c r="K4" s="8">
-        <v>-0.95459000000000005</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.13492000000000001</v>
-      </c>
-      <c r="M4" s="8">
-        <v>2.9203000000000001</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1.2495000000000001</v>
-      </c>
-      <c r="O4" s="8">
-        <v>2.9472999999999998</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1.2231000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1.5431999999999999</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.81201999999999996</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3.0230999999999999</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.72885999999999995</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-1.2414000000000001</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.23852000000000001</v>
-      </c>
-      <c r="G5" s="5">
-        <v>2.2831999999999999</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.70816000000000001</v>
-      </c>
-      <c r="I5" s="1">
-        <v>3.7734999999999999</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.72851999999999995</v>
-      </c>
-      <c r="K5" s="8">
-        <v>-0.98540000000000005</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.13211999999999999</v>
-      </c>
-      <c r="M5" s="8">
-        <v>3.2942</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1.03</v>
-      </c>
-      <c r="O5" s="8">
-        <v>4.3425000000000002</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1.0053000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1.4343999999999999</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.93140999999999996</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.9561000000000002</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.87287000000000003</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-1.2482</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.27481</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2.1953</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.83811000000000002</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3.6974999999999998</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.87441000000000002</v>
-      </c>
-      <c r="K6" s="8">
-        <v>-0.94411999999999996</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.12615999999999999</v>
-      </c>
-      <c r="M6" s="8">
-        <v>2.8203</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1.3335999999999999</v>
-      </c>
-      <c r="O6" s="8">
-        <v>3.8673000000000002</v>
-      </c>
-      <c r="P6" s="2">
-        <v>1.3140000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <f>AVERAGE(A4:A6)</f>
-        <v>1.4521333333333333</v>
-      </c>
-      <c r="B7" s="6">
-        <f t="shared" ref="B7:P7" si="0">AVERAGE(B4:B6)</f>
-        <v>0.87586333333333333</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" si="0"/>
-        <v>2.9543666666666666</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.81627666666666665</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.2450333333333334</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.25768666666666667</v>
-      </c>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>2.2033</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.78463333333333329</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>3.6988666666666661</v>
-      </c>
-      <c r="J7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.81636333333333333</v>
-      </c>
-      <c r="K7" s="6">
-        <f t="shared" si="0"/>
-        <v>-0.96137000000000006</v>
-      </c>
-      <c r="L7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.13106666666666666</v>
-      </c>
-      <c r="M7" s="6">
-        <f t="shared" si="0"/>
-        <v>3.0116000000000001</v>
-      </c>
-      <c r="N7" s="6">
-        <f t="shared" si="0"/>
-        <v>1.2043666666666668</v>
-      </c>
-      <c r="O7" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7190333333333334</v>
-      </c>
-      <c r="P7" s="6">
-        <f t="shared" si="0"/>
-        <v>1.1808000000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E7DF8D5-E926-4ED6-B61D-79F53C888D0D}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -9166,19 +8869,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -9302,12 +9005,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B558B864-F812-42EE-9431-77FDE3BF624C}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9317,19 +9020,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -9433,7 +9136,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>